<commit_message>
maaping updated and custom sort corrected
</commit_message>
<xml_diff>
--- a/Car_type_Mapping/mapping details.xlsx
+++ b/Car_type_Mapping/mapping details.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rail car\Car_type_Mapping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rail_car_trace_app\railcar_trace_automation\rail_car\Car_type_Mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B73C2F-91FD-4399-834C-1A72B2DD5547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A8A59E-BF95-404C-932D-F64C7635FEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9A6BAA09-B97B-4C91-8EC3-5AE4875C12CA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9A6BAA09-B97B-4C91-8EC3-5AE4875C12CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>Commodity Name</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>CORN</t>
+  </si>
+  <si>
+    <t>COTTONSEED NBXC</t>
+  </si>
+  <si>
+    <t>SOYBN CK ML SCR</t>
   </si>
 </sst>
 </file>
@@ -615,11 +621,14 @@
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -980,10 +989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F050650-30A7-431A-B1C3-203E3BF595AA}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,46 +1043,62 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new required changes made
</commit_message>
<xml_diff>
--- a/Car_type_Mapping/mapping details.xlsx
+++ b/Car_type_Mapping/mapping details.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rail_car_trace_app\railcar_trace_automation\rail_car\Car_type_Mapping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rail car\Car_type_Mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A8A59E-BF95-404C-932D-F64C7635FEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311D73B9-1428-427F-B390-AB114C1804F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9A6BAA09-B97B-4C91-8EC3-5AE4875C12CA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9A6BAA09-B97B-4C91-8EC3-5AE4875C12CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Commodity Name</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>SOYBN CK ML SCR</t>
+  </si>
+  <si>
+    <t>Inbound YC Reload HRW</t>
   </si>
 </sst>
 </file>
@@ -621,14 +624,11 @@
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -992,7 +992,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,7 +1045,7 @@
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1066,8 +1066,8 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>11</v>
+      <c r="A9" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>11</v>
@@ -1090,8 +1090,8 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>14</v>
+      <c r="A12" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>14</v>
@@ -1102,5 +1102,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
completed dev as on 05-10-2023
</commit_message>
<xml_diff>
--- a/Car_type_Mapping/mapping details.xlsx
+++ b/Car_type_Mapping/mapping details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rail car\Car_type_Mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311D73B9-1428-427F-B390-AB114C1804F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164883AD-0F08-4834-9761-8B478CCAF0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9A6BAA09-B97B-4C91-8EC3-5AE4875C12CA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Commodity Name</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>Inbound YC Reload HRW</t>
+  </si>
+  <si>
+    <t>OILS,NUT,SEED</t>
+  </si>
+  <si>
+    <t>PALM OIL</t>
   </si>
 </sst>
 </file>
@@ -624,9 +630,8 @@
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -992,7 +997,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,103 +1007,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
+      <c r="A13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changes for color code
</commit_message>
<xml_diff>
--- a/Car_type_Mapping/mapping details.xlsx
+++ b/Car_type_Mapping/mapping details.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rail car\Car_type_Mapping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rail_car_trace_app\railcar_trace_automation\rail_car\Car_type_Mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A6DE1D-6FDC-40FF-AAF1-0D767F0F6C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434595C5-A292-4418-9A8E-D83AA824C7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{9A6BAA09-B97B-4C91-8EC3-5AE4875C12CA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9A6BAA09-B97B-4C91-8EC3-5AE4875C12CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Commodity Name</t>
   </si>
@@ -92,20 +92,26 @@
     <t>Inbound YC Reload HRW</t>
   </si>
   <si>
+    <t>CK/ML RAPE SEED</t>
+  </si>
+  <si>
     <t>OILS,NUT,SEED</t>
   </si>
   <si>
-    <t>PALM OIL</t>
+    <t>Palm Oil</t>
   </si>
   <si>
     <t>OILS NUT SEED</t>
+  </si>
+  <si>
+    <t>DIST MASH SPT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,6 +261,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -443,7 +457,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -588,8 +602,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -632,9 +657,11 @@
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -642,8 +669,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -677,6 +707,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink 2" xfId="42" xr:uid="{AE0929DC-2921-4D7C-8676-DAD20F57A953}"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -997,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F050650-30A7-431A-B1C3-203E3BF595AA}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,115 +1041,139 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B13" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="3" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>20</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>